<commit_message>
update command & excel
</commit_message>
<xml_diff>
--- a/tags.xlsx
+++ b/tags.xlsx
@@ -20,7 +20,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t xml:space="preserve">name file</t>
+  </si>
   <si>
     <t xml:space="preserve">eiffel.jpg</t>
   </si>
@@ -131,39 +134,41 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="H7" activeCellId="0" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="B2" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="n">
+      <c r="C2" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="0" t="n">
         <v>123</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="0" t="s">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="B3" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="0" t="n">
         <v>878</v>
       </c>
     </row>

</xml_diff>